<commit_message>
Add all fakequake branches
</commit_message>
<xml_diff>
--- a/data/branch_weight_data.xlsx
+++ b/data/branch_weight_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmc753\Work\occ-coseismic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12FBF4B-C2C4-45D3-9C25-F8F68D7A5FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2FBA37-4859-4760-BB8F-F5754AFB47AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all sheets" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="280">
   <si>
     <t>N</t>
   </si>
@@ -843,12 +843,6 @@
     <t>_py_M5NQ</t>
   </si>
   <si>
-    <t>_sz_fq_1</t>
-  </si>
-  <si>
-    <t>sz_solutions/FakeQuakes_sz_n5000_S10_N1_GR100_b1-1_N21-5_nIt500000_narchi10</t>
-  </si>
-  <si>
     <t>_sz_Njk2</t>
   </si>
   <si>
@@ -868,6 +862,24 @@
   </si>
   <si>
     <t>ti</t>
+  </si>
+  <si>
+    <t>sz_solutions/FakeQuakes_sz_n5000_S10_N1_GR500_b0-95_N16-5_nIt1000000_narchi10</t>
+  </si>
+  <si>
+    <t>sz_solutions/FakeQuakes_sz_n5000_S10_N1_GR500_b1-1_N21-5_nIt1000000_narchi10</t>
+  </si>
+  <si>
+    <t>sz_solutions/FakeQuakes_sz_n5000_S10_N1_GR500_b1-24_N27-9_nIt1000000_narchi10</t>
+  </si>
+  <si>
+    <t>_sz_fq_b095</t>
+  </si>
+  <si>
+    <t>_sz_fq_b110</t>
+  </si>
+  <si>
+    <t>_sz_fq_b124</t>
   </si>
 </sst>
 </file>
@@ -6754,7 +6766,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="J2" sqref="J2:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6858,10 +6870,10 @@
         <v>3.685658469623871E-2</v>
       </c>
       <c r="M2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="N2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -6905,7 +6917,7 @@
         <v>1.9298622376880636E-2</v>
       </c>
       <c r="M3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -6949,7 +6961,7 @@
         <v>1.9449984121013036E-2</v>
       </c>
       <c r="M4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -6993,10 +7005,10 @@
         <v>0.16947599171126124</v>
       </c>
       <c r="M5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="N5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -7040,7 +7052,7 @@
         <v>8.873999565990065E-2</v>
       </c>
       <c r="M6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -7084,7 +7096,7 @@
         <v>8.9435995625860659E-2</v>
       </c>
       <c r="M7" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -7128,10 +7140,10 @@
         <v>0.28115491107998747</v>
       </c>
       <c r="M8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="N8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -7175,7 +7187,7 @@
         <v>0.14721663721847394</v>
       </c>
       <c r="M9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -7219,7 +7231,7 @@
         <v>0.14837127751038354</v>
       </c>
       <c r="M10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -7230,10 +7242,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C3AB27-DA22-46B6-9275-CBA251195A6D}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7296,12 +7308,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21.5</v>
+        <v>27.9</v>
       </c>
       <c r="B2">
-        <v>1.097</v>
+        <v>1.24</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -7316,39 +7328,39 @@
         <v>260</v>
       </c>
       <c r="G2">
-        <v>0.45212999999999998</v>
+        <v>0.20552999999999999</v>
       </c>
       <c r="H2">
         <v>0.48699999999999999</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I4" si="0">PRODUCT(G2:H2)</f>
-        <v>0.22018730999999997</v>
+        <f>PRODUCT(G2:H2)</f>
+        <v>0.10009311</v>
       </c>
       <c r="J2">
-        <v>1.2753645444283894E-4</v>
+        <v>6.1013978779008275E-5</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K4" si="1">J2*I2</f>
-        <v>2.8081908830706253E-5</v>
+        <f>J2*I2</f>
+        <v>6.107078889464941E-6</v>
       </c>
       <c r="L2">
-        <f>K2/(SUM(K$2:K$4))</f>
-        <v>0.48748748748748749</v>
+        <f>K2/(SUM(K$8:K$16))</f>
+        <v>6.3904712892699972E-2</v>
       </c>
       <c r="M2" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="N2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>21.5</v>
+        <v>27.9</v>
       </c>
       <c r="B3">
-        <v>1.097</v>
+        <v>1.24</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -7363,36 +7375,36 @@
         <v>260</v>
       </c>
       <c r="G3">
-        <v>0.45212999999999998</v>
+        <v>0.20552999999999999</v>
       </c>
       <c r="H3">
         <v>0.255</v>
       </c>
       <c r="I3">
-        <f t="shared" si="0"/>
-        <v>0.11529315</v>
+        <f>PRODUCT(G3:H3)</f>
+        <v>5.2410149999999996E-2</v>
       </c>
       <c r="J3">
-        <v>1.2753645444283894E-4</v>
+        <v>6.1013978779008275E-5</v>
       </c>
       <c r="K3">
-        <f t="shared" si="1"/>
-        <v>1.4704079572546396E-5</v>
+        <f>J3*I3</f>
+        <v>3.1977517799046403E-6</v>
       </c>
       <c r="L3">
-        <f>K3/(SUM(K$2:K$4))</f>
-        <v>0.25525525525525528</v>
+        <f>K3/(SUM(K$8:K$16))</f>
+        <v>3.3461399974617029E-2</v>
       </c>
       <c r="M3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>21.5</v>
+        <v>27.9</v>
       </c>
       <c r="B4">
-        <v>1.097</v>
+        <v>1.24</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -7407,31 +7419,302 @@
         <v>260</v>
       </c>
       <c r="G4">
-        <v>0.45212999999999998</v>
+        <v>0.20552999999999999</v>
       </c>
       <c r="H4">
         <v>0.25700000000000001</v>
       </c>
       <c r="I4">
+        <f>PRODUCT(G4:H4)</f>
+        <v>5.282121E-2</v>
+      </c>
+      <c r="J4">
+        <v>6.1013978779008275E-5</v>
+      </c>
+      <c r="K4">
+        <f>J4*I4</f>
+        <v>3.2228321860215396E-6</v>
+      </c>
+      <c r="L4">
+        <f>K4/(SUM(K$8:K$16))</f>
+        <v>3.3723842327359123E-2</v>
+      </c>
+      <c r="M4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>21.5</v>
+      </c>
+      <c r="B5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>257</v>
+      </c>
+      <c r="F5" t="s">
+        <v>260</v>
+      </c>
+      <c r="G5">
+        <v>0.45212999999999998</v>
+      </c>
+      <c r="H5">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="I5">
+        <f>PRODUCT(G5:H5)</f>
+        <v>0.22018730999999997</v>
+      </c>
+      <c r="J5">
+        <v>1.2753645444283894E-4</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K7" si="0">J5*I5</f>
+        <v>2.8081908830706253E-5</v>
+      </c>
+      <c r="L5">
+        <f>K5/(SUM(K$8:K$16))</f>
+        <v>0.29385019479623692</v>
+      </c>
+      <c r="M5" t="s">
+        <v>278</v>
+      </c>
+      <c r="N5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>21.5</v>
+      </c>
+      <c r="B6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0.42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>257</v>
+      </c>
+      <c r="F6" t="s">
+        <v>260</v>
+      </c>
+      <c r="G6">
+        <v>0.45212999999999998</v>
+      </c>
+      <c r="H6">
+        <v>0.255</v>
+      </c>
+      <c r="I6">
+        <f>PRODUCT(G6:H6)</f>
+        <v>0.11529315</v>
+      </c>
+      <c r="J6">
+        <v>1.2753645444283894E-4</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="0"/>
+        <v>1.4704079572546396E-5</v>
+      </c>
+      <c r="L6">
+        <f>K6/(SUM(K$8:K$16))</f>
+        <v>0.15386406503704397</v>
+      </c>
+      <c r="M6" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>21.5</v>
+      </c>
+      <c r="B7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>1.58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>257</v>
+      </c>
+      <c r="F7" t="s">
+        <v>260</v>
+      </c>
+      <c r="G7">
+        <v>0.45212999999999998</v>
+      </c>
+      <c r="H7">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="I7">
+        <f>PRODUCT(G7:H7)</f>
         <v>0.11619741</v>
       </c>
-      <c r="J4">
+      <c r="J7">
         <v>1.2753645444283894E-4</v>
       </c>
-      <c r="K4">
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>1.4819405686840878E-5</v>
+      </c>
+      <c r="L7">
+        <f>K7/(SUM(K$8:K$16))</f>
+        <v>0.15507084201772667</v>
+      </c>
+      <c r="M7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>16.5</v>
+      </c>
+      <c r="B8">
+        <v>0.95</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>257</v>
+      </c>
+      <c r="F8" t="s">
+        <v>260</v>
+      </c>
+      <c r="G8">
+        <v>0.34233999999999998</v>
+      </c>
+      <c r="H8">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ref="I8:I16" si="1">PRODUCT(G8:H8)</f>
+        <v>0.16671957999999998</v>
+      </c>
+      <c r="J8">
+        <v>2.7943288043777702E-4</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ref="K8:K10" si="2">J8*I8</f>
+        <v>4.6586932464776397E-5</v>
+      </c>
+      <c r="L8">
+        <f>K8/(SUM(K$8:K$16))</f>
+        <v>0.48748748748748744</v>
+      </c>
+      <c r="M8" t="s">
+        <v>277</v>
+      </c>
+      <c r="N8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>16.5</v>
+      </c>
+      <c r="B9">
+        <v>0.95</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>0.42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>257</v>
+      </c>
+      <c r="F9" t="s">
+        <v>260</v>
+      </c>
+      <c r="G9">
+        <v>0.34233999999999998</v>
+      </c>
+      <c r="H9">
+        <v>0.255</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="1"/>
-        <v>1.4819405686840878E-5</v>
-      </c>
-      <c r="L4">
-        <f>K4/(SUM(K$2:K$4))</f>
+        <v>8.7296699999999991E-2</v>
+      </c>
+      <c r="J9">
+        <v>2.7943288043777702E-4</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>2.4393568333712488E-5</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ref="L9:L16" si="3">K9/(SUM(K$8:K$16))</f>
+        <v>0.25525525525525522</v>
+      </c>
+      <c r="M9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>16.5</v>
+      </c>
+      <c r="B10">
+        <v>0.95</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>1.58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>257</v>
+      </c>
+      <c r="F10" t="s">
+        <v>260</v>
+      </c>
+      <c r="G10">
+        <v>0.34233999999999998</v>
+      </c>
+      <c r="H10">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>8.7981379999999998E-2</v>
+      </c>
+      <c r="J10">
+        <v>2.7943288043777702E-4</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>2.4584890438290627E-5</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="3"/>
         <v>0.25725725725725729</v>
       </c>
-      <c r="M4" t="s">
-        <v>267</v>
+      <c r="M10" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7440,7 +7723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E83D2B-8D51-4F58-8B18-609D52F42AB5}">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -7521,7 +7804,7 @@
         <v>142</v>
       </c>
       <c r="F2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G2">
         <v>0.48599999999999999</v>
@@ -7575,7 +7858,7 @@
         <v>142</v>
       </c>
       <c r="F3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G3">
         <v>0.48599999999999999</v>
@@ -7626,7 +7909,7 @@
         <v>142</v>
       </c>
       <c r="F4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G4">
         <v>0.48599999999999999</v>

</xml_diff>

<commit_message>
69 write out single branches (#71)
* Remove repetitions in defining datafiles

* Allow single branches to be written out to QGIS

* Add FQ branches
</commit_message>
<xml_diff>
--- a/data/branch_weight_data.xlsx
+++ b/data/branch_weight_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmc753\Work\occ-coseismic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7205C966-937E-4212-9015-90B14F0A8DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71E1D78-769F-4C4E-AF49-A343480665EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all sheets" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="292">
   <si>
     <t>N</t>
   </si>
@@ -880,6 +880,42 @@
   </si>
   <si>
     <t>_sz_fq_b124</t>
+  </si>
+  <si>
+    <t>_sz_fq_3nub11</t>
+  </si>
+  <si>
+    <t>sz_solutions/FakeQuakes_hk_3e10_nolocking_uniformSlip_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
+  </si>
+  <si>
+    <t>sz_solutions/FakeQuakes_hk_prem_nolocking_uniformSlip_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
+  </si>
+  <si>
+    <t>_sz_fq_pnub11</t>
+  </si>
+  <si>
+    <t>sz_solutions/FakeQuakes_hk_prem_nolocking_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
+  </si>
+  <si>
+    <t>sz_solutions/FakeQuakes_hk_3e10_locking_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
+  </si>
+  <si>
+    <t>sz_solutions/FakeQuakes_hk_prem_locking_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
+  </si>
+  <si>
+    <t>_sz_fq_3nb110</t>
+  </si>
+  <si>
+    <t>_sz_fq_pnb110</t>
+  </si>
+  <si>
+    <t>_sz_fq_3lb110</t>
+  </si>
+  <si>
+    <t>_sz_fq_plb110</t>
+  </si>
+  <si>
+    <t>sz_solutions/FakeQuakes_hk_3e10_nolocking_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
   </si>
 </sst>
 </file>
@@ -2874,6 +2910,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 Classification: In-Confidence</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -4194,6 +4233,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 Classification: In-Confidence</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -6185,6 +6227,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 Classification: In-Confidence</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -6758,6 +6803,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 Classification: In-Confidence</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -7237,15 +7285,18 @@
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 Classification: In-Confidence</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C3AB27-DA22-46B6-9275-CBA251195A6D}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="K11" sqref="K11:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7345,8 +7396,8 @@
         <v>6.107078889464941E-6</v>
       </c>
       <c r="L2">
-        <f>K2/(SUM(K$2:K$10))</f>
-        <v>3.685658469623871E-2</v>
+        <f>K2/(SUM(K$2:K$50))</f>
+        <v>1.8274277194337614E-2</v>
       </c>
       <c r="M2" t="s">
         <v>279</v>
@@ -7392,8 +7443,8 @@
         <v>3.1977517799046403E-6</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L10" si="1">K3/(SUM(K$2:K$10))</f>
-        <v>1.9298622376880636E-2</v>
+        <f t="shared" ref="L3:L12" si="1">K3/(SUM(K$2:K$50))</f>
+        <v>9.5686667034005982E-3</v>
       </c>
       <c r="M3" t="s">
         <v>279</v>
@@ -7437,7 +7488,7 @@
       </c>
       <c r="L4">
         <f t="shared" si="1"/>
-        <v>1.9449984121013036E-2</v>
+        <v>9.6437150697017797E-3</v>
       </c>
       <c r="M4" t="s">
         <v>279</v>
@@ -7481,7 +7532,7 @@
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>0.16947599171126124</v>
+        <v>8.4029794834270463E-2</v>
       </c>
       <c r="M5" t="s">
         <v>278</v>
@@ -7528,7 +7579,7 @@
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
-        <v>8.873999565990065E-2</v>
+        <v>4.3999173886527659E-2</v>
       </c>
       <c r="M6" t="s">
         <v>278</v>
@@ -7572,7 +7623,7 @@
       </c>
       <c r="L7">
         <f t="shared" si="1"/>
-        <v>8.9435995625860659E-2</v>
+        <v>4.4344265446421997E-2</v>
       </c>
       <c r="M7" t="s">
         <v>278</v>
@@ -7604,19 +7655,19 @@
         <v>0.48699999999999999</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:I10" si="3">PRODUCT(G8:H8)</f>
+        <f t="shared" ref="I8:I11" si="3">PRODUCT(G8:H8)</f>
         <v>0.16671957999999998</v>
       </c>
       <c r="J8">
         <v>2.7943288043777702E-4</v>
       </c>
       <c r="K8">
-        <f t="shared" ref="K8:K10" si="4">J8*I8</f>
+        <f t="shared" ref="K8:K11" si="4">J8*I8</f>
         <v>4.6586932464776397E-5</v>
       </c>
       <c r="L8">
         <f t="shared" si="1"/>
-        <v>0.28115491107998747</v>
+        <v>0.13940257411179413</v>
       </c>
       <c r="M8" t="s">
         <v>277</v>
@@ -7663,7 +7714,7 @@
       </c>
       <c r="L9">
         <f t="shared" si="1"/>
-        <v>0.14721663721847394</v>
+        <v>7.2993134288516434E-2</v>
       </c>
       <c r="M9" t="s">
         <v>277</v>
@@ -7707,15 +7758,300 @@
       </c>
       <c r="L10">
         <f t="shared" si="1"/>
-        <v>0.14837127751038354</v>
+        <v>7.356562945940677E-2</v>
       </c>
       <c r="M10" t="s">
         <v>277</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>21.5</v>
+      </c>
+      <c r="B11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>257</v>
+      </c>
+      <c r="F11" t="s">
+        <v>260</v>
+      </c>
+      <c r="G11">
+        <v>0.45212999999999998</v>
+      </c>
+      <c r="H11">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>0.22018730999999997</v>
+      </c>
+      <c r="J11">
+        <v>1.2753645444283894E-4</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>2.8081908830706253E-5</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>8.4029794834270463E-2</v>
+      </c>
+      <c r="M11" t="s">
+        <v>280</v>
+      </c>
+      <c r="N11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>21.5</v>
+      </c>
+      <c r="B12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>257</v>
+      </c>
+      <c r="F12" t="s">
+        <v>260</v>
+      </c>
+      <c r="G12">
+        <v>0.45212999999999998</v>
+      </c>
+      <c r="H12">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12" si="5">PRODUCT(G12:H12)</f>
+        <v>0.22018730999999997</v>
+      </c>
+      <c r="J12">
+        <v>1.2753645444283894E-4</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ref="K12" si="6">J12*I12</f>
+        <v>2.8081908830706253E-5</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>8.4029794834270463E-2</v>
+      </c>
+      <c r="M12" t="s">
+        <v>283</v>
+      </c>
+      <c r="N12" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>21.5</v>
+      </c>
+      <c r="B13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>257</v>
+      </c>
+      <c r="F13" t="s">
+        <v>260</v>
+      </c>
+      <c r="G13">
+        <v>0.45212999999999998</v>
+      </c>
+      <c r="H13">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ref="I13:I15" si="7">PRODUCT(G13:H13)</f>
+        <v>0.22018730999999997</v>
+      </c>
+      <c r="J13">
+        <v>1.2753645444283894E-4</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ref="K13:K15" si="8">J13*I13</f>
+        <v>2.8081908830706253E-5</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ref="L13:L15" si="9">K13/(SUM(K$2:K$50))</f>
+        <v>8.4029794834270463E-2</v>
+      </c>
+      <c r="M13" t="s">
+        <v>287</v>
+      </c>
+      <c r="N13" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>21.5</v>
+      </c>
+      <c r="B14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>257</v>
+      </c>
+      <c r="F14" t="s">
+        <v>260</v>
+      </c>
+      <c r="G14">
+        <v>0.45212999999999998</v>
+      </c>
+      <c r="H14">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="7"/>
+        <v>0.22018730999999997</v>
+      </c>
+      <c r="J14">
+        <v>1.2753645444283894E-4</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="8"/>
+        <v>2.8081908830706253E-5</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="9"/>
+        <v>8.4029794834270463E-2</v>
+      </c>
+      <c r="M14" t="s">
+        <v>288</v>
+      </c>
+      <c r="N14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>21.5</v>
+      </c>
+      <c r="B15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>257</v>
+      </c>
+      <c r="F15" t="s">
+        <v>260</v>
+      </c>
+      <c r="G15">
+        <v>0.45212999999999998</v>
+      </c>
+      <c r="H15">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="7"/>
+        <v>0.22018730999999997</v>
+      </c>
+      <c r="J15">
+        <v>1.2753645444283894E-4</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="8"/>
+        <v>2.8081908830706253E-5</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="9"/>
+        <v>8.4029794834270463E-2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>289</v>
+      </c>
+      <c r="N15" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>21.5</v>
+      </c>
+      <c r="B16">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>257</v>
+      </c>
+      <c r="F16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G16">
+        <v>0.45212999999999998</v>
+      </c>
+      <c r="H16">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ref="I16" si="10">PRODUCT(G16:H16)</f>
+        <v>0.22018730999999997</v>
+      </c>
+      <c r="J16">
+        <v>1.2753645444283894E-4</v>
+      </c>
+      <c r="K16">
+        <f t="shared" ref="K16" si="11">J16*I16</f>
+        <v>2.8081908830706253E-5</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ref="L16" si="12">K16/(SUM(K$2:K$50))</f>
+        <v>8.4029794834270463E-2</v>
+      </c>
+      <c r="M16" t="s">
+        <v>290</v>
+      </c>
+      <c r="N16" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 Classification: In-Confidence</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -7945,6 +8281,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 Classification: In-Confidence</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -8278,5 +8617,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 Classification: In-Confidence</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add more fq outputs
</commit_message>
<xml_diff>
--- a/data/branch_weight_data.xlsx
+++ b/data/branch_weight_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmc753\Work\occ-coseismic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71E1D78-769F-4C4E-AF49-A343480665EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011CEAD3-87E0-463C-9943-FEC2A1750E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all sheets" sheetId="1" r:id="rId1"/>
@@ -882,18 +882,12 @@
     <t>_sz_fq_b124</t>
   </si>
   <si>
-    <t>_sz_fq_3nub11</t>
-  </si>
-  <si>
     <t>sz_solutions/FakeQuakes_hk_3e10_nolocking_uniformSlip_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
   </si>
   <si>
     <t>sz_solutions/FakeQuakes_hk_prem_nolocking_uniformSlip_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
   </si>
   <si>
-    <t>_sz_fq_pnub11</t>
-  </si>
-  <si>
     <t>sz_solutions/FakeQuakes_hk_prem_nolocking_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
   </si>
   <si>
@@ -903,19 +897,25 @@
     <t>sz_solutions/FakeQuakes_hk_prem_locking_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
   </si>
   <si>
-    <t>_sz_fq_3nb110</t>
-  </si>
-  <si>
-    <t>_sz_fq_pnb110</t>
-  </si>
-  <si>
-    <t>_sz_fq_3lb110</t>
-  </si>
-  <si>
-    <t>_sz_fq_plb110</t>
-  </si>
-  <si>
     <t>sz_solutions/FakeQuakes_hk_3e10_nolocking_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
+  </si>
+  <si>
+    <t>_sz_fq_3nhb110</t>
+  </si>
+  <si>
+    <t>_sz_fq_pnhb110</t>
+  </si>
+  <si>
+    <t>_sz_fq_3lhb110</t>
+  </si>
+  <si>
+    <t>_sz_fq_plhb110</t>
+  </si>
+  <si>
+    <t>_sz_fq_pnub110</t>
+  </si>
+  <si>
+    <t>_sz_fq_3nub110</t>
   </si>
 </sst>
 </file>
@@ -7296,7 +7296,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:K16"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7805,10 +7805,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M11" t="s">
+        <v>291</v>
+      </c>
+      <c r="N11" t="s">
         <v>280</v>
-      </c>
-      <c r="N11" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -7852,10 +7852,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M12" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="N12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -7899,10 +7899,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="N13" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -7946,10 +7946,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -7993,10 +7993,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N15" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -8040,10 +8040,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="N16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow multiple defined single branches
</commit_message>
<xml_diff>
--- a/data/branch_weight_data.xlsx
+++ b/data/branch_weight_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmc753\Work\occ-coseismic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71E1D78-769F-4C4E-AF49-A343480665EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD03881-87D5-40A4-9B76-B215E2EB6BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all sheets" sheetId="1" r:id="rId1"/>
@@ -882,18 +882,12 @@
     <t>_sz_fq_b124</t>
   </si>
   <si>
-    <t>_sz_fq_3nub11</t>
-  </si>
-  <si>
     <t>sz_solutions/FakeQuakes_hk_3e10_nolocking_uniformSlip_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
   </si>
   <si>
     <t>sz_solutions/FakeQuakes_hk_prem_nolocking_uniformSlip_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
   </si>
   <si>
-    <t>_sz_fq_pnub11</t>
-  </si>
-  <si>
     <t>sz_solutions/FakeQuakes_hk_prem_nolocking_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
   </si>
   <si>
@@ -903,19 +897,25 @@
     <t>sz_solutions/FakeQuakes_hk_prem_locking_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
   </si>
   <si>
-    <t>_sz_fq_3nb110</t>
-  </si>
-  <si>
-    <t>_sz_fq_pnb110</t>
-  </si>
-  <si>
-    <t>_sz_fq_3lb110</t>
-  </si>
-  <si>
-    <t>_sz_fq_plb110</t>
-  </si>
-  <si>
     <t>sz_solutions/FakeQuakes_hk_3e10_nolocking_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
+  </si>
+  <si>
+    <t>_sz_fq_3nub110</t>
+  </si>
+  <si>
+    <t>_sz_fq_pnub110</t>
+  </si>
+  <si>
+    <t>_sz_fq_3nhb110</t>
+  </si>
+  <si>
+    <t>_sz_fq_pnhb110</t>
+  </si>
+  <si>
+    <t>_sz_fq_3lhb110</t>
+  </si>
+  <si>
+    <t>_sz_fq_plhb110</t>
   </si>
 </sst>
 </file>
@@ -7296,7 +7296,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:K16"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7805,10 +7805,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M11" t="s">
+        <v>286</v>
+      </c>
+      <c r="N11" t="s">
         <v>280</v>
-      </c>
-      <c r="N11" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -7852,10 +7852,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M12" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="N12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -7899,10 +7899,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M13" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="N13" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -7946,10 +7946,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M14" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="N14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -7993,10 +7993,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M15" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="N15" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -8040,10 +8040,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M16" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="N16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
75 plot transects (#76)
* Allow multiple defined single branches

* Declutter potentially useful but unused scripts

* Output min-max in errors as well

* Add scripts for comparing single fault branches

* Add explainer RSt file for documentation

* Improved labelling
</commit_message>
<xml_diff>
--- a/data/branch_weight_data.xlsx
+++ b/data/branch_weight_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmc753\Work\occ-coseismic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71E1D78-769F-4C4E-AF49-A343480665EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD03881-87D5-40A4-9B76-B215E2EB6BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all sheets" sheetId="1" r:id="rId1"/>
@@ -882,18 +882,12 @@
     <t>_sz_fq_b124</t>
   </si>
   <si>
-    <t>_sz_fq_3nub11</t>
-  </si>
-  <si>
     <t>sz_solutions/FakeQuakes_hk_3e10_nolocking_uniformSlip_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
   </si>
   <si>
     <t>sz_solutions/FakeQuakes_hk_prem_nolocking_uniformSlip_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
   </si>
   <si>
-    <t>_sz_fq_pnub11</t>
-  </si>
-  <si>
     <t>sz_solutions/FakeQuakes_hk_prem_nolocking_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
   </si>
   <si>
@@ -903,19 +897,25 @@
     <t>sz_solutions/FakeQuakes_hk_prem_locking_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
   </si>
   <si>
-    <t>_sz_fq_3nb110</t>
-  </si>
-  <si>
-    <t>_sz_fq_pnb110</t>
-  </si>
-  <si>
-    <t>_sz_fq_3lb110</t>
-  </si>
-  <si>
-    <t>_sz_fq_plb110</t>
-  </si>
-  <si>
     <t>sz_solutions/FakeQuakes_hk_3e10_nolocking_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
+  </si>
+  <si>
+    <t>_sz_fq_3nub110</t>
+  </si>
+  <si>
+    <t>_sz_fq_pnub110</t>
+  </si>
+  <si>
+    <t>_sz_fq_3nhb110</t>
+  </si>
+  <si>
+    <t>_sz_fq_pnhb110</t>
+  </si>
+  <si>
+    <t>_sz_fq_3lhb110</t>
+  </si>
+  <si>
+    <t>_sz_fq_plhb110</t>
   </si>
 </sst>
 </file>
@@ -7296,7 +7296,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:K16"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7805,10 +7805,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M11" t="s">
+        <v>286</v>
+      </c>
+      <c r="N11" t="s">
         <v>280</v>
-      </c>
-      <c r="N11" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -7852,10 +7852,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M12" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="N12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -7899,10 +7899,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M13" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="N13" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -7946,10 +7946,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M14" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="N14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -7993,10 +7993,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M15" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="N15" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -8040,10 +8040,10 @@
         <v>8.4029794834270463E-2</v>
       </c>
       <c r="M16" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="N16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to files to work on
</commit_message>
<xml_diff>
--- a/data/branch_weight_data.xlsx
+++ b/data/branch_weight_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\McGrath\occ-coseismic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9220C6-3EEF-4ABC-91DF-FB735891B757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0F0579-7CEF-4670-896A-4E09145F3E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="286">
   <si>
     <t>N</t>
   </si>
@@ -862,24 +862,6 @@
   </si>
   <si>
     <t>ti</t>
-  </si>
-  <si>
-    <t>sz_solutions/FakeQuakes_sz_n5000_S10_N1_GR500_b0-95_N16-5_nIt1000000_narchi10</t>
-  </si>
-  <si>
-    <t>sz_solutions/FakeQuakes_sz_n5000_S10_N1_GR500_b1-1_N21-5_nIt1000000_narchi10</t>
-  </si>
-  <si>
-    <t>sz_solutions/FakeQuakes_sz_n5000_S10_N1_GR500_b1-24_N27-9_nIt1000000_narchi10</t>
-  </si>
-  <si>
-    <t>_sz_fq_b095</t>
-  </si>
-  <si>
-    <t>_sz_fq_b110</t>
-  </si>
-  <si>
-    <t>_sz_fq_b124</t>
   </si>
   <si>
     <t>sz_solutions/FakeQuakes_hk_3e10_nolocking_uniformSlip_n5000_S10_N1_GR500_b1-1_N21-5_nIt500000_narchi10</t>
@@ -7293,10 +7275,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C3AB27-DA22-46B6-9275-CBA251195A6D}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7359,12 +7341,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>27.9</v>
+        <v>21.5</v>
       </c>
       <c r="B2">
-        <v>1.24</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -7379,45 +7361,45 @@
         <v>260</v>
       </c>
       <c r="G2">
-        <v>0.20552999999999999</v>
+        <v>0.45212999999999998</v>
       </c>
       <c r="H2">
         <v>0.48699999999999999</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I7" si="0">PRODUCT(G2:H2)</f>
-        <v>0.10009311</v>
+        <f t="shared" ref="I2" si="0">PRODUCT(G2:H2)</f>
+        <v>0.22018730999999997</v>
       </c>
       <c r="J2">
-        <v>6.1013978779008275E-5</v>
+        <v>1.2753645444283894E-4</v>
       </c>
       <c r="K2">
-        <f>J2*I2</f>
-        <v>6.107078889464941E-6</v>
+        <f t="shared" ref="K2" si="1">J2*I2</f>
+        <v>2.8081908830706253E-5</v>
       </c>
       <c r="L2">
-        <f>K2/(SUM(K$2:K$50))</f>
-        <v>1.8274277194337614E-2</v>
+        <f>K2/(SUM(K$2:K$41))</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="M2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="N2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>27.9</v>
+        <v>21.5</v>
       </c>
       <c r="B3">
-        <v>1.24</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="D3">
-        <v>0.42</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>257</v>
@@ -7426,42 +7408,45 @@
         <v>260</v>
       </c>
       <c r="G3">
-        <v>0.20552999999999999</v>
+        <v>0.45212999999999998</v>
       </c>
       <c r="H3">
-        <v>0.255</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="I3">
-        <f t="shared" si="0"/>
-        <v>5.2410149999999996E-2</v>
+        <f t="shared" ref="I3" si="2">PRODUCT(G3:H3)</f>
+        <v>0.22018730999999997</v>
       </c>
       <c r="J3">
-        <v>6.1013978779008275E-5</v>
+        <v>1.2753645444283894E-4</v>
       </c>
       <c r="K3">
-        <f>J3*I3</f>
-        <v>3.1977517799046403E-6</v>
+        <f t="shared" ref="K3" si="3">J3*I3</f>
+        <v>2.8081908830706253E-5</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L12" si="1">K3/(SUM(K$2:K$50))</f>
-        <v>9.5686667034005982E-3</v>
+        <f>K3/(SUM(K$2:K$41))</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="M3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+      <c r="N3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>27.9</v>
+        <v>21.5</v>
       </c>
       <c r="B4">
-        <v>1.24</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4">
-        <v>1.58</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>257</v>
@@ -7470,31 +7455,34 @@
         <v>260</v>
       </c>
       <c r="G4">
-        <v>0.20552999999999999</v>
+        <v>0.45212999999999998</v>
       </c>
       <c r="H4">
-        <v>0.25700000000000001</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>5.282121E-2</v>
+        <f t="shared" ref="I4:I6" si="4">PRODUCT(G4:H4)</f>
+        <v>0.22018730999999997</v>
       </c>
       <c r="J4">
-        <v>6.1013978779008275E-5</v>
+        <v>1.2753645444283894E-4</v>
       </c>
       <c r="K4">
-        <f>J4*I4</f>
-        <v>3.2228321860215396E-6</v>
+        <f t="shared" ref="K4:K6" si="5">J4*I4</f>
+        <v>2.8081908830706253E-5</v>
       </c>
       <c r="L4">
-        <f t="shared" si="1"/>
-        <v>9.6437150697017797E-3</v>
+        <f>K4/(SUM(K$2:K$41))</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="M4" t="s">
+        <v>282</v>
+      </c>
+      <c r="N4" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>21.5</v>
       </c>
@@ -7520,28 +7508,28 @@
         <v>0.48699999999999999</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.22018730999999997</v>
       </c>
       <c r="J5">
         <v>1.2753645444283894E-4</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:K7" si="2">J5*I5</f>
+        <f t="shared" si="5"/>
         <v>2.8081908830706253E-5</v>
       </c>
       <c r="L5">
-        <f t="shared" si="1"/>
-        <v>8.4029794834270463E-2</v>
+        <f>K5/(SUM(K$2:K$41))</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="M5" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="N5" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>21.5</v>
       </c>
@@ -7552,7 +7540,7 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>0.42</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>257</v>
@@ -7564,28 +7552,31 @@
         <v>0.45212999999999998</v>
       </c>
       <c r="H6">
-        <v>0.255</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
-        <v>0.11529315</v>
+        <f t="shared" si="4"/>
+        <v>0.22018730999999997</v>
       </c>
       <c r="J6">
         <v>1.2753645444283894E-4</v>
       </c>
       <c r="K6">
-        <f t="shared" si="2"/>
-        <v>1.4704079572546396E-5</v>
+        <f t="shared" si="5"/>
+        <v>2.8081908830706253E-5</v>
       </c>
       <c r="L6">
-        <f t="shared" si="1"/>
-        <v>4.3999173886527659E-2</v>
+        <f>K6/(SUM(K$2:K$41))</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="M6" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="N6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>21.5</v>
       </c>
@@ -7596,7 +7587,7 @@
         <v>4</v>
       </c>
       <c r="D7">
-        <v>1.58</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>257</v>
@@ -7608,442 +7599,28 @@
         <v>0.45212999999999998</v>
       </c>
       <c r="H7">
-        <v>0.25700000000000001</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
-        <v>0.11619741</v>
+        <f t="shared" ref="I7" si="6">PRODUCT(G7:H7)</f>
+        <v>0.22018730999999997</v>
       </c>
       <c r="J7">
         <v>1.2753645444283894E-4</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
-        <v>1.4819405686840878E-5</v>
+        <f t="shared" ref="K7" si="7">J7*I7</f>
+        <v>2.8081908830706253E-5</v>
       </c>
       <c r="L7">
-        <f t="shared" si="1"/>
-        <v>4.4344265446421997E-2</v>
+        <f>K7/(SUM(K$2:K$41))</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="M7" t="s">
+        <v>285</v>
+      </c>
+      <c r="N7" t="s">
         <v>278</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>16.5</v>
-      </c>
-      <c r="B8">
-        <v>0.95</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>257</v>
-      </c>
-      <c r="F8" t="s">
-        <v>260</v>
-      </c>
-      <c r="G8">
-        <v>0.34233999999999998</v>
-      </c>
-      <c r="H8">
-        <v>0.48699999999999999</v>
-      </c>
-      <c r="I8">
-        <f t="shared" ref="I8:I11" si="3">PRODUCT(G8:H8)</f>
-        <v>0.16671957999999998</v>
-      </c>
-      <c r="J8">
-        <v>2.7943288043777702E-4</v>
-      </c>
-      <c r="K8">
-        <f t="shared" ref="K8:K11" si="4">J8*I8</f>
-        <v>4.6586932464776397E-5</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="1"/>
-        <v>0.13940257411179413</v>
-      </c>
-      <c r="M8" t="s">
-        <v>277</v>
-      </c>
-      <c r="N8" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>16.5</v>
-      </c>
-      <c r="B9">
-        <v>0.95</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>0.42</v>
-      </c>
-      <c r="E9" t="s">
-        <v>257</v>
-      </c>
-      <c r="F9" t="s">
-        <v>260</v>
-      </c>
-      <c r="G9">
-        <v>0.34233999999999998</v>
-      </c>
-      <c r="H9">
-        <v>0.255</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="3"/>
-        <v>8.7296699999999991E-2</v>
-      </c>
-      <c r="J9">
-        <v>2.7943288043777702E-4</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="4"/>
-        <v>2.4393568333712488E-5</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="1"/>
-        <v>7.2993134288516434E-2</v>
-      </c>
-      <c r="M9" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>16.5</v>
-      </c>
-      <c r="B10">
-        <v>0.95</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>1.58</v>
-      </c>
-      <c r="E10" t="s">
-        <v>257</v>
-      </c>
-      <c r="F10" t="s">
-        <v>260</v>
-      </c>
-      <c r="G10">
-        <v>0.34233999999999998</v>
-      </c>
-      <c r="H10">
-        <v>0.25700000000000001</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="3"/>
-        <v>8.7981379999999998E-2</v>
-      </c>
-      <c r="J10">
-        <v>2.7943288043777702E-4</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="4"/>
-        <v>2.4584890438290627E-5</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="1"/>
-        <v>7.356562945940677E-2</v>
-      </c>
-      <c r="M10" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>21.5</v>
-      </c>
-      <c r="B11">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>257</v>
-      </c>
-      <c r="F11" t="s">
-        <v>260</v>
-      </c>
-      <c r="G11">
-        <v>0.45212999999999998</v>
-      </c>
-      <c r="H11">
-        <v>0.48699999999999999</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="3"/>
-        <v>0.22018730999999997</v>
-      </c>
-      <c r="J11">
-        <v>1.2753645444283894E-4</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="4"/>
-        <v>2.8081908830706253E-5</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="1"/>
-        <v>8.4029794834270463E-2</v>
-      </c>
-      <c r="M11" t="s">
-        <v>286</v>
-      </c>
-      <c r="N11" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>21.5</v>
-      </c>
-      <c r="B12">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>257</v>
-      </c>
-      <c r="F12" t="s">
-        <v>260</v>
-      </c>
-      <c r="G12">
-        <v>0.45212999999999998</v>
-      </c>
-      <c r="H12">
-        <v>0.48699999999999999</v>
-      </c>
-      <c r="I12">
-        <f t="shared" ref="I12" si="5">PRODUCT(G12:H12)</f>
-        <v>0.22018730999999997</v>
-      </c>
-      <c r="J12">
-        <v>1.2753645444283894E-4</v>
-      </c>
-      <c r="K12">
-        <f t="shared" ref="K12" si="6">J12*I12</f>
-        <v>2.8081908830706253E-5</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="1"/>
-        <v>8.4029794834270463E-2</v>
-      </c>
-      <c r="M12" t="s">
-        <v>287</v>
-      </c>
-      <c r="N12" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>21.5</v>
-      </c>
-      <c r="B13">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C13">
-        <v>4</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>257</v>
-      </c>
-      <c r="F13" t="s">
-        <v>260</v>
-      </c>
-      <c r="G13">
-        <v>0.45212999999999998</v>
-      </c>
-      <c r="H13">
-        <v>0.48699999999999999</v>
-      </c>
-      <c r="I13">
-        <f t="shared" ref="I13:I15" si="7">PRODUCT(G13:H13)</f>
-        <v>0.22018730999999997</v>
-      </c>
-      <c r="J13">
-        <v>1.2753645444283894E-4</v>
-      </c>
-      <c r="K13">
-        <f t="shared" ref="K13:K15" si="8">J13*I13</f>
-        <v>2.8081908830706253E-5</v>
-      </c>
-      <c r="L13">
-        <f t="shared" ref="L13:L15" si="9">K13/(SUM(K$2:K$50))</f>
-        <v>8.4029794834270463E-2</v>
-      </c>
-      <c r="M13" t="s">
-        <v>288</v>
-      </c>
-      <c r="N13" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>21.5</v>
-      </c>
-      <c r="B14">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>257</v>
-      </c>
-      <c r="F14" t="s">
-        <v>260</v>
-      </c>
-      <c r="G14">
-        <v>0.45212999999999998</v>
-      </c>
-      <c r="H14">
-        <v>0.48699999999999999</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="7"/>
-        <v>0.22018730999999997</v>
-      </c>
-      <c r="J14">
-        <v>1.2753645444283894E-4</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="8"/>
-        <v>2.8081908830706253E-5</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="9"/>
-        <v>8.4029794834270463E-2</v>
-      </c>
-      <c r="M14" t="s">
-        <v>289</v>
-      </c>
-      <c r="N14" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>21.5</v>
-      </c>
-      <c r="B15">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C15">
-        <v>4</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>257</v>
-      </c>
-      <c r="F15" t="s">
-        <v>260</v>
-      </c>
-      <c r="G15">
-        <v>0.45212999999999998</v>
-      </c>
-      <c r="H15">
-        <v>0.48699999999999999</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="7"/>
-        <v>0.22018730999999997</v>
-      </c>
-      <c r="J15">
-        <v>1.2753645444283894E-4</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="8"/>
-        <v>2.8081908830706253E-5</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="9"/>
-        <v>8.4029794834270463E-2</v>
-      </c>
-      <c r="M15" t="s">
-        <v>290</v>
-      </c>
-      <c r="N15" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>21.5</v>
-      </c>
-      <c r="B16">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>257</v>
-      </c>
-      <c r="F16" t="s">
-        <v>260</v>
-      </c>
-      <c r="G16">
-        <v>0.45212999999999998</v>
-      </c>
-      <c r="H16">
-        <v>0.48699999999999999</v>
-      </c>
-      <c r="I16">
-        <f t="shared" ref="I16" si="10">PRODUCT(G16:H16)</f>
-        <v>0.22018730999999997</v>
-      </c>
-      <c r="J16">
-        <v>1.2753645444283894E-4</v>
-      </c>
-      <c r="K16">
-        <f t="shared" ref="K16" si="11">J16*I16</f>
-        <v>2.8081908830706253E-5</v>
-      </c>
-      <c r="L16">
-        <f t="shared" ref="L16" si="12">K16/(SUM(K$2:K$50))</f>
-        <v>8.4029794834270463E-2</v>
-      </c>
-      <c r="M16" t="s">
-        <v>291</v>
-      </c>
-      <c r="N16" t="s">
-        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>